<commit_message>
Modification de la création des formules et de la création d'une estimation
</commit_message>
<xml_diff>
--- a/.temp/planning.xlsx
+++ b/.temp/planning.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEV_QUALICOM\Desktop\Remi\dev\chezmessoeurs\.temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\programmation\Qualicom\chezmessoeurs\.temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99446817-1BB0-49A6-ACD6-A594206496B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="57">
   <si>
     <t>Réalisé</t>
   </si>
@@ -70,9 +69,6 @@
   </si>
   <si>
     <t>archiver</t>
-  </si>
-  <si>
-    <t>en cours</t>
   </si>
   <si>
     <t>vue estimations</t>
@@ -204,7 +200,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -522,11 +518,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,10 +535,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -561,24 +557,24 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1">
         <v>43893</v>
@@ -587,14 +583,14 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="1">
         <v>43894</v>
@@ -603,14 +599,14 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1">
         <v>43900</v>
@@ -619,33 +615,33 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="1">
         <v>43899</v>
@@ -658,10 +654,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1">
         <v>43899</v>
@@ -670,14 +666,14 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="1">
         <v>43899</v>
@@ -686,14 +682,14 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" s="1">
         <v>43899</v>
@@ -706,10 +702,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1">
         <v>43899</v>
@@ -722,25 +718,25 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1">
         <v>43899</v>
@@ -749,14 +745,14 @@
         <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1">
         <v>43899</v>
@@ -765,14 +761,14 @@
         <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="1">
         <v>43899</v>
@@ -781,7 +777,7 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -792,13 +788,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" s="1">
         <v>43901</v>
@@ -828,7 +824,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -873,23 +869,23 @@
         <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D34" s="1">
         <v>43901</v>
@@ -911,7 +907,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -945,7 +941,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>15</v>
+        <v>53</v>
+      </c>
+      <c r="D43" s="1">
+        <v>43907</v>
       </c>
       <c r="E43" t="s">
         <v>7</v>
@@ -989,7 +988,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
@@ -1000,7 +999,7 @@
         <v>7</v>
       </c>
       <c r="G49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="4:7" x14ac:dyDescent="0.25">
@@ -1011,7 +1010,7 @@
         <v>7</v>
       </c>
       <c r="G50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="4:7" x14ac:dyDescent="0.25">
@@ -1019,12 +1018,12 @@
         <v>7</v>
       </c>
       <c r="G51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="4:7" x14ac:dyDescent="0.25">
@@ -1040,7 +1039,7 @@
         <v>10</v>
       </c>
       <c r="G55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="4:7" x14ac:dyDescent="0.25">
@@ -1048,7 +1047,7 @@
         <v>7</v>
       </c>
       <c r="G56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57" spans="4:7" x14ac:dyDescent="0.25">
@@ -1077,7 +1076,7 @@
     </row>
     <row r="61" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="4:7" x14ac:dyDescent="0.25">
@@ -1085,7 +1084,7 @@
         <v>7</v>
       </c>
       <c r="G62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="4:7" x14ac:dyDescent="0.25">
@@ -1093,7 +1092,7 @@
         <v>7</v>
       </c>
       <c r="G63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="4:7" x14ac:dyDescent="0.25">
@@ -1101,7 +1100,7 @@
         <v>7</v>
       </c>
       <c r="G64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.25">
@@ -1109,12 +1108,12 @@
         <v>10</v>
       </c>
       <c r="G65" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.25">
@@ -1162,7 +1161,7 @@
         <v>10</v>
       </c>
       <c r="G73" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="74" spans="5:7" x14ac:dyDescent="0.25">
@@ -1170,12 +1169,12 @@
         <v>10</v>
       </c>
       <c r="G74" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="76" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F76" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="77" spans="5:7" x14ac:dyDescent="0.25">
@@ -1183,7 +1182,7 @@
         <v>10</v>
       </c>
       <c r="G77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="5:7" x14ac:dyDescent="0.25">
@@ -1191,7 +1190,7 @@
         <v>10</v>
       </c>
       <c r="G78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="79" spans="5:7" x14ac:dyDescent="0.25">
@@ -1199,12 +1198,12 @@
         <v>10</v>
       </c>
       <c r="G79" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F81" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82" spans="5:7" x14ac:dyDescent="0.25">
@@ -1212,7 +1211,7 @@
         <v>10</v>
       </c>
       <c r="G82" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="83" spans="5:7" x14ac:dyDescent="0.25">
@@ -1220,7 +1219,7 @@
         <v>10</v>
       </c>
       <c r="G83" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="84" spans="5:7" x14ac:dyDescent="0.25">
@@ -1228,12 +1227,12 @@
         <v>10</v>
       </c>
       <c r="G84" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="86" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="87" spans="5:7" x14ac:dyDescent="0.25">
@@ -1241,7 +1240,7 @@
         <v>10</v>
       </c>
       <c r="G87" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
avancement sur devis. Affichage d'un devis en cours
</commit_message>
<xml_diff>
--- a/.temp/planning.xlsx
+++ b/.temp/planning.xlsx
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,7 +940,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+      <c r="C43" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D43" s="1">
@@ -954,6 +954,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="3"/>
       <c r="D44" s="1">
         <v>43900</v>
       </c>
@@ -965,6 +966,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="3"/>
       <c r="D45" s="1">
         <v>43900</v>
       </c>
@@ -976,6 +978,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="3"/>
       <c r="D46" s="1">
         <v>43900</v>
       </c>
@@ -1244,11 +1247,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B7:B17"/>
     <mergeCell ref="A7:A17"/>
+    <mergeCell ref="C43:C46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
correction typo  front js devisitem pour 'Pièce Salée' -> 'Pièce salée'
</commit_message>
<xml_diff>
--- a/.temp/planning.xlsx
+++ b/.temp/planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="57">
   <si>
     <t>Réalisé</t>
   </si>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="K67" sqref="K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,7 +994,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="D49" s="1">
         <v>43900</v>
       </c>
@@ -1005,7 +1008,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C50" s="3"/>
       <c r="D50" s="1">
         <v>43900</v>
       </c>
@@ -1016,7 +1020,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C51" s="3"/>
+      <c r="D51" s="1">
+        <v>43917</v>
+      </c>
       <c r="E51" t="s">
         <v>7</v>
       </c>
@@ -1024,12 +1032,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C54" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D54" s="1">
+        <v>43917</v>
+      </c>
       <c r="E54" t="s">
         <v>7</v>
       </c>
@@ -1037,7 +1051,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C55" s="3"/>
+      <c r="D55" s="1">
+        <v>43917</v>
+      </c>
       <c r="E55" t="s">
         <v>10</v>
       </c>
@@ -1045,7 +1063,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C56" s="3"/>
+      <c r="D56" s="1">
+        <v>43917</v>
+      </c>
       <c r="E56" t="s">
         <v>7</v>
       </c>
@@ -1053,7 +1075,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C57" s="3"/>
+      <c r="D57" s="1">
+        <v>43917</v>
+      </c>
       <c r="E57" t="s">
         <v>7</v>
       </c>
@@ -1061,7 +1087,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C58" s="3"/>
+      <c r="D58" s="1">
+        <v>43917</v>
+      </c>
       <c r="E58" t="s">
         <v>7</v>
       </c>
@@ -1069,7 +1099,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C59" s="3"/>
+      <c r="D59" s="1">
+        <v>43917</v>
+      </c>
       <c r="E59" t="s">
         <v>10</v>
       </c>
@@ -1077,12 +1111,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F61" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C62" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" s="1">
+        <v>43917</v>
+      </c>
       <c r="E62" t="s">
         <v>7</v>
       </c>
@@ -1090,7 +1130,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C63" s="3"/>
+      <c r="D63" s="1">
+        <v>43917</v>
+      </c>
       <c r="E63" t="s">
         <v>7</v>
       </c>
@@ -1098,7 +1142,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C64" s="3"/>
+      <c r="D64" s="1">
+        <v>43917</v>
+      </c>
       <c r="E64" t="s">
         <v>7</v>
       </c>
@@ -1106,7 +1154,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C65" s="3"/>
+      <c r="D65" s="1">
+        <v>43917</v>
+      </c>
       <c r="E65" t="s">
         <v>10</v>
       </c>
@@ -1114,12 +1166,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
         <v>10</v>
       </c>
@@ -1127,7 +1179,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
         <v>10</v>
       </c>
@@ -1135,7 +1187,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
         <v>10</v>
       </c>
@@ -1143,7 +1195,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
         <v>10</v>
       </c>
@@ -1151,7 +1203,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
         <v>10</v>
       </c>
@@ -1159,7 +1211,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
         <v>10</v>
       </c>
@@ -1167,7 +1219,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
         <v>10</v>
       </c>
@@ -1175,12 +1227,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F76" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
         <v>10</v>
       </c>
@@ -1188,7 +1240,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
         <v>10</v>
       </c>
@@ -1196,7 +1248,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
         <v>10</v>
       </c>
@@ -1247,7 +1299,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="C62:C65"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B7:B17"/>

</xml_diff>